<commit_message>
update to only show unlabelled rows
</commit_message>
<xml_diff>
--- a/assets/data/Crowdsourced_normal_2k_rs42.xlsx
+++ b/assets/data/Crowdsourced_normal_2k_rs42.xlsx
@@ -6328,7 +6328,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6339,7 +6339,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6350,7 +6350,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -6361,7 +6361,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>